<commit_message>
Export PE sudah oke
</commit_message>
<xml_diff>
--- a/public/discipline-assesment/Contoh Import Disiplin.xlsx
+++ b/public/discipline-assesment/Contoh Import Disiplin.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
     <t xml:space="preserve">Bulan</t>
   </si>
@@ -43,7 +43,10 @@
     <t xml:space="preserve">Terlambat</t>
   </si>
   <si>
-    <t xml:space="preserve">EN-4-086</t>
+    <t xml:space="preserve">EN-4-046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agus Priyanto</t>
   </si>
   <si>
     <t xml:space="preserve">Abdul Fikri</t>
@@ -266,7 +269,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -319,7 +322,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -333,7 +336,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="6" t="n">
         <v>1</v>
@@ -356,7 +359,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="6" t="n">
         <v>0</v>
@@ -379,7 +382,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="6" t="n">
         <v>0</v>
@@ -402,7 +405,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="6" t="n">
         <v>0</v>
@@ -425,7 +428,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="6" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Perbaikan dikit di QPE
</commit_message>
<xml_diff>
--- a/public/discipline-assesment/Contoh Import Disiplin.xlsx
+++ b/public/discipline-assesment/Contoh Import Disiplin.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t xml:space="preserve">Bulan</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t xml:space="preserve">Agus Priyanto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abdul Fikri</t>
   </si>
 </sst>
 </file>
@@ -269,7 +266,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -336,7 +333,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="6" t="n">
         <v>1</v>
@@ -359,7 +356,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="6" t="n">
         <v>0</v>
@@ -382,7 +379,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="6" t="n">
         <v>0</v>
@@ -405,7 +402,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="6" t="n">
         <v>0</v>
@@ -428,7 +425,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="6" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Pop Up Panduan Skala Behavior
</commit_message>
<xml_diff>
--- a/public/discipline-assesment/Contoh Import Disiplin.xlsx
+++ b/public/discipline-assesment/Contoh Import Disiplin.xlsx
@@ -43,10 +43,10 @@
     <t xml:space="preserve">Terlambat</t>
   </si>
   <si>
-    <t xml:space="preserve">EN-4-046</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agus Priyanto</t>
+    <t xml:space="preserve">EN-4-047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ari Pratama</t>
   </si>
 </sst>
 </file>
@@ -266,7 +266,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Menampilkan total grade skala 4 dan fitur upload Evidence
</commit_message>
<xml_diff>
--- a/public/discipline-assesment/Contoh Import Disiplin.xlsx
+++ b/public/discipline-assesment/Contoh Import Disiplin.xlsx
@@ -43,10 +43,10 @@
     <t xml:space="preserve">Terlambat</t>
   </si>
   <si>
-    <t xml:space="preserve">EN-4-047</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ari Pratama </t>
+    <t xml:space="preserve">EN-4-046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agus Priyanto</t>
   </si>
 </sst>
 </file>

</xml_diff>